<commit_message>
Adding the new work on R class.
</commit_message>
<xml_diff>
--- a/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
+++ b/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
@@ -5,19 +5,19 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Miller/GitHub/GhNanoDegree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Miller/GitHub/DAnanodegree/A_Overall_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26320" yWindow="1680" windowWidth="24820" windowHeight="13940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="860" yWindow="1680" windowWidth="24740" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Schedule" sheetId="1" r:id="rId1"/>
-    <sheet name="Milestones" sheetId="2" r:id="rId2"/>
-    <sheet name="Time Spent" sheetId="3" r:id="rId3"/>
+    <sheet name="Milestones" sheetId="2" r:id="rId1"/>
+    <sheet name="Time Spent" sheetId="3" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Time Spent'!$A$4:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Time Spent'!$A$4:$C$4</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
   <si>
     <t>Nanodegree - Data Analyst</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>Data Wrangling Project</t>
+  </si>
+  <si>
+    <t>Data Wrangling Project - Finished</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,7 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -554,7 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -567,6 +569,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -866,240 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,13 +890,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1256,8 +1032,8 @@
       <c r="C12" s="9">
         <v>42333</v>
       </c>
-      <c r="D12" s="24">
-        <v>0.1</v>
+      <c r="D12" s="20">
+        <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>45</v>
@@ -1273,8 +1049,8 @@
       <c r="C13" s="9">
         <v>42347</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>61</v>
+      <c r="D13" s="20">
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>43</v>
@@ -1290,8 +1066,8 @@
       <c r="C14" s="9">
         <v>75259</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>61</v>
+      <c r="D14" s="29">
+        <v>0.1</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>47</v>
@@ -1456,214 +1232,205 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
       <c r="E31" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
       <c r="E35" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="188" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
       <c r="E36" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="199" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
       <c r="E39" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
       <c r="E40" s="16" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
       <c r="E41" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
       <c r="E42" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="16" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A33:D33"/>
@@ -1674,6 +1441,15 @@
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1682,12 +1458,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1709,7 +1485,7 @@
       </c>
       <c r="B2" s="13">
         <f>SUM(B5:B400)</f>
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2674,7 +2450,7 @@
       <c r="B144" s="12">
         <v>2</v>
       </c>
-      <c r="C144" s="25" t="s">
+      <c r="C144" s="24" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2685,7 +2461,7 @@
       <c r="B145" s="12">
         <v>2</v>
       </c>
-      <c r="C145" s="25" t="s">
+      <c r="C145" s="24" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2696,7 +2472,7 @@
       <c r="B146" s="12">
         <v>5</v>
       </c>
-      <c r="C146" s="25" t="s">
+      <c r="C146" s="24" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2734,15 +2510,33 @@
       <c r="A153" s="14">
         <v>42350</v>
       </c>
+      <c r="B153" s="12">
+        <v>8</v>
+      </c>
+      <c r="C153" s="25" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="14">
         <v>42351</v>
       </c>
+      <c r="B154" s="12">
+        <v>6</v>
+      </c>
+      <c r="C154" s="25" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="14">
         <v>42352</v>
+      </c>
+      <c r="B155" s="12">
+        <v>2</v>
+      </c>
+      <c r="C155" s="25" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -2842,4 +2636,234 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating my Github to reflect mid-progress through ML.
</commit_message>
<xml_diff>
--- a/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
+++ b/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1680" windowWidth="24740" windowHeight="13940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1020" yWindow="1340" windowWidth="24740" windowHeight="13940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Milestones" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>Nanodegree - Data Analyst</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>Worked on R EDA Project</t>
+  </si>
+  <si>
+    <t>Worked on R EDA Project - Review Comments</t>
+  </si>
+  <si>
+    <t>Starting Machine Learning</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -588,12 +594,75 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -905,13 +974,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1446,15 +1515,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A33:D33"/>
@@ -1465,6 +1525,15 @@
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1477,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1500,7 +1569,7 @@
       </c>
       <c r="B2" s="13">
         <f>SUM(B5:B400)</f>
-        <v>159</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2771,6 +2840,12 @@
       <c r="A189" s="14">
         <v>42386</v>
       </c>
+      <c r="B189" s="30">
+        <v>2</v>
+      </c>
+      <c r="C189" s="30" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="14">
@@ -2787,82 +2862,100 @@
         <v>42389</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="14">
         <v>42390</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="14">
         <v>42391</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="14">
         <v>42392</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B195" s="30">
+        <v>5</v>
+      </c>
+      <c r="C195" s="30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="14">
         <v>42393</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B196" s="30">
+        <v>4</v>
+      </c>
+      <c r="C196" s="30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="14">
         <v>42394</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B197" s="12">
+        <v>1</v>
+      </c>
+      <c r="C197" s="30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="14">
         <v>42395</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="14">
         <v>42396</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="14">
         <v>42397</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="14">
         <v>42398</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="14">
         <v>42399</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="14">
         <v>42400</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="14">
         <v>42401</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="14">
         <v>42402</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="14">
         <v>42403</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="14">
         <v>42404</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="14">
         <v>42405</v>
       </c>
@@ -2947,162 +3040,183 @@
         <v>42421</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="14">
         <v>42422</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B225" s="12">
+        <v>3</v>
+      </c>
+      <c r="C225" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="14">
         <v>42423</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="14">
         <v>42424</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="14">
         <v>42425</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="14">
         <v>42426</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="14">
         <v>42427</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="14">
         <v>42428</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="14">
         <v>42429</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="14">
         <v>42430</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="14">
         <v>42431</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="14">
         <v>42432</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="14">
         <v>42433</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="14">
         <v>42434</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B237" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="14">
         <v>42435</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B238" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="14">
         <v>42436</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="14">
         <v>42437</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="14">
         <v>42438</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="14">
         <v>42439</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="14">
         <v>42440</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="14">
         <v>42441</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="14">
         <v>42442</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B245" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="14">
         <v>42443</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="14">
         <v>42444</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="14">
         <v>42445</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="14">
         <v>42446</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="14">
         <v>42447</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="14">
         <v>42448</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B251" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="14">
         <v>42449</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B252" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="14">
         <v>42450</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="14">
         <v>42451</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="14">
         <v>42452</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="14">
         <v>42453</v>
       </c>
@@ -3344,12 +3458,36 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:C4"/>
-  <conditionalFormatting sqref="B5:B357">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="B5:B188 B190:B194 B197:B357">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B189">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B195">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B196">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating my Github to reflect progress on Final project
</commit_message>
<xml_diff>
--- a/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
+++ b/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="110">
   <si>
     <t>Nanodegree - Data Analyst</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Starting Machine Learning</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Machine Learning - PCA</t>
   </si>
 </sst>
 </file>
@@ -522,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -588,14 +594,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,13 +983,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="136" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1316,205 +1325,214 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="213" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="16" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="E29" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
       <c r="E30" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
       <c r="E35" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="188" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="199" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
       <c r="E38" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="16" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
       <c r="E42" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
       <c r="E43" s="16" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="A33:D33"/>
@@ -1525,15 +1543,6 @@
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
@@ -1546,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="C252" sqref="C252"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C260" sqref="C260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,7 +1578,7 @@
       </c>
       <c r="B2" s="13">
         <f>SUM(B5:B400)</f>
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3113,6 +3122,9 @@
       <c r="B237" s="12">
         <v>1</v>
       </c>
+      <c r="C237" s="12" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="14">
@@ -3121,6 +3133,9 @@
       <c r="B238" s="12">
         <v>4</v>
       </c>
+      <c r="C238" s="31" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="14">
@@ -3132,171 +3147,192 @@
         <v>42437</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="14">
         <v>42438</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="14">
         <v>42439</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="14">
         <v>42440</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="14">
         <v>42441</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="14">
         <v>42442</v>
       </c>
       <c r="B245" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C245" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="14">
         <v>42443</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="14">
         <v>42444</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="14">
         <v>42445</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="14">
         <v>42446</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="14">
         <v>42447</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="14">
         <v>42448</v>
       </c>
       <c r="B251" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C251" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="14">
         <v>42449</v>
       </c>
       <c r="B252" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="C252" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="14">
         <v>42450</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B253" s="12">
+        <v>2</v>
+      </c>
+      <c r="C253" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="14">
         <v>42451</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="14">
         <v>42452</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="14">
         <v>42453</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="14">
         <v>42454</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="14">
         <v>42455</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="14">
         <v>42456</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="14">
         <v>42457</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B260" s="12">
+        <v>4</v>
+      </c>
+      <c r="C260" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="14">
         <v>42458</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="14">
         <v>42459</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="14">
         <v>42460</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="14">
         <v>42461</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="14">
         <v>42462</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="14">
         <v>42463</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="14">
         <v>42464</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="14">
         <v>42465</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="14">
         <v>42466</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="14">
         <v>42467</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="14">
         <v>42468</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="14">
         <v>42469</v>
       </c>

</xml_diff>

<commit_message>
Pushed Final P5 for evaluation by Udacity.
</commit_message>
<xml_diff>
--- a/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
+++ b/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
@@ -15,13 +15,14 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Time Spent'!$A$4:$C$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Time Spent'!$A$4:$C$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Time Spent'!$A$4:$C$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="111">
   <si>
     <t>Nanodegree (https://www.udacity.com/course/data-analyst-nanodegree--nd002)</t>
   </si>
@@ -549,7 +550,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -640,6 +641,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -861,7 +866,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="C265 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1460,8 +1465,8 @@
   </sheetPr>
   <dimension ref="A1:C303"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B264" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C266" activeCellId="0" sqref="C266"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A263" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C265" activeCellId="0" sqref="C265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1485,7 +1490,7 @@
       </c>
       <c r="B2" s="19" t="n">
         <f aca="false">SUM(B5:B400)</f>
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C2" s="0"/>
     </row>
@@ -3571,35 +3576,49 @@
       <c r="A261" s="20" t="n">
         <v>42458</v>
       </c>
+      <c r="B261" s="0"/>
+      <c r="C261" s="0"/>
     </row>
     <row r="262" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="20" t="n">
         <v>42459</v>
       </c>
+      <c r="B262" s="0"/>
+      <c r="C262" s="0"/>
     </row>
     <row r="263" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="20" t="n">
         <v>42460</v>
       </c>
+      <c r="B263" s="0"/>
+      <c r="C263" s="0"/>
     </row>
     <row r="264" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="20" t="n">
         <v>42461</v>
       </c>
+      <c r="B264" s="0"/>
+      <c r="C264" s="0"/>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="20" t="n">
         <v>42462</v>
       </c>
+      <c r="B265" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C265" s="23" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="20" t="n">
         <v>42463</v>
       </c>
-      <c r="B266" s="16" t="n">
+      <c r="B266" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="C266" s="16" t="s">
+      <c r="C266" s="23" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3607,40 +3626,56 @@
       <c r="A267" s="20" t="n">
         <v>42464</v>
       </c>
+      <c r="B267" s="0"/>
+      <c r="C267" s="0"/>
     </row>
     <row r="268" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="20" t="n">
         <v>42465</v>
       </c>
+      <c r="B268" s="0"/>
+      <c r="C268" s="0"/>
     </row>
     <row r="269" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="20" t="n">
         <v>42466</v>
       </c>
+      <c r="B269" s="0"/>
+      <c r="C269" s="0"/>
     </row>
     <row r="270" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="20" t="n">
         <v>42467</v>
       </c>
+      <c r="B270" s="0"/>
+      <c r="C270" s="0"/>
     </row>
     <row r="271" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="20" t="n">
         <v>42468</v>
       </c>
-    </row>
-    <row r="272" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B271" s="0"/>
+      <c r="C271" s="0"/>
+    </row>
+    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="20" t="n">
         <v>42469</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C272" s="23" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="20" t="n">
         <v>42470</v>
       </c>
-      <c r="B273" s="16" t="n">
+      <c r="B273" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="C273" s="16" t="s">
+      <c r="C273" s="23" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3648,30 +3683,38 @@
       <c r="A274" s="20" t="n">
         <v>42471</v>
       </c>
+      <c r="B274" s="0"/>
+      <c r="C274" s="0"/>
     </row>
     <row r="275" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="20" t="n">
         <v>42472</v>
       </c>
+      <c r="B275" s="0"/>
+      <c r="C275" s="0"/>
     </row>
     <row r="276" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="20" t="n">
         <v>42473</v>
       </c>
+      <c r="B276" s="0"/>
+      <c r="C276" s="0"/>
     </row>
     <row r="277" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="20" t="n">
         <v>42474</v>
       </c>
+      <c r="B277" s="0"/>
+      <c r="C277" s="0"/>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="20" t="n">
         <v>42475</v>
       </c>
-      <c r="B278" s="16" t="n">
+      <c r="B278" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="C278" s="16" t="s">
+      <c r="C278" s="23" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3679,10 +3722,10 @@
       <c r="A279" s="20" t="n">
         <v>42476</v>
       </c>
-      <c r="B279" s="16" t="n">
-        <v>6</v>
-      </c>
-      <c r="C279" s="16" t="s">
+      <c r="B279" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="C279" s="23" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3808,7 +3851,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:C4"/>
-  <conditionalFormatting sqref="B5:B188,B190:B194,B197:B357">
+  <conditionalFormatting sqref="B189">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -3816,7 +3859,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B189">
+  <conditionalFormatting sqref="B195">
     <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>0</formula>
     </cfRule>
@@ -3824,19 +3867,11 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B195">
+  <conditionalFormatting sqref="B196">
     <cfRule type="cellIs" priority="6" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" priority="7" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B196">
-    <cfRule type="cellIs" priority="8" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="9" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3859,7 +3894,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="C265 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -3874,7 +3909,7 @@
       <c r="E1" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="23"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="0" t="s">
         <v>86</v>
       </c>
@@ -3883,39 +3918,39 @@
       <c r="A2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="26" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>97</v>
       </c>
       <c r="B5" s="6"/>
@@ -3927,127 +3962,127 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="26"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="26"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>100</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>104</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="26" t="s">
         <v>106</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>107</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="26" t="s">
         <v>108</v>
       </c>
       <c r="B16" s="6"/>
@@ -4055,11 +4090,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="26"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>109</v>
       </c>
       <c r="B17" s="6"/>
@@ -4071,7 +4106,7 @@
       <c r="H17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>110</v>
       </c>
       <c r="B18" s="6"/>

</xml_diff>

<commit_message>
P6 - Data Visualization - Post Udacity Reviewer and many more revisions
</commit_message>
<xml_diff>
--- a/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
+++ b/A_Overall_Documents/NanoDegree_Overview_Milestones.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="116">
   <si>
     <t>Nanodegree (https://www.udacity.com/course/data-analyst-nanodegree--nd002)</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>weeks</t>
+  </si>
+  <si>
+    <t>AB Testing</t>
+  </si>
+  <si>
+    <t>Fixing Data Visualization Project</t>
   </si>
 </sst>
 </file>
@@ -1598,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK365"/>
+  <dimension ref="A1:AMK366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1624,12 +1630,12 @@
         <v>51</v>
       </c>
       <c r="B2" s="16">
-        <f>SUM(B5:B900)</f>
-        <v>263</v>
+        <f>SUM(B5:B901)</f>
+        <v>273</v>
       </c>
       <c r="C2">
         <f>B2/40</f>
-        <v>6.5750000000000002</v>
+        <v>6.8250000000000002</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>113</v>
@@ -4052,7 +4058,7 @@
         <v>42504</v>
       </c>
       <c r="B307" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C307" s="13" t="s">
         <v>112</v>
@@ -4062,289 +4068,312 @@
       <c r="A308" s="17">
         <v>42505</v>
       </c>
+      <c r="B308" s="13">
+        <v>2</v>
+      </c>
+      <c r="C308" s="13" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="17">
-        <v>42506</v>
+        <v>42505</v>
+      </c>
+      <c r="B309" s="13">
+        <v>1</v>
+      </c>
+      <c r="C309" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="17">
-        <v>42507</v>
+        <v>42506</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="17">
-        <v>42508</v>
+        <v>42507</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="17">
-        <v>42509</v>
+        <v>42508</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="17">
-        <v>42510</v>
+        <v>42509</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="17">
-        <v>42511</v>
+        <v>42510</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="17">
-        <v>42512</v>
+        <v>42511</v>
+      </c>
+      <c r="B315" s="13">
+        <v>6</v>
+      </c>
+      <c r="C315" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="17">
-        <v>42513</v>
+        <v>42512</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="17">
-        <v>42514</v>
+        <v>42513</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="17">
-        <v>42515</v>
+        <v>42514</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="17">
-        <v>42516</v>
+        <v>42515</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="17">
-        <v>42517</v>
+        <v>42516</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="17">
-        <v>42518</v>
+        <v>42517</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="17">
-        <v>42519</v>
+        <v>42518</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="17">
-        <v>42520</v>
+        <v>42519</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="17">
-        <v>42521</v>
+        <v>42520</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="17">
-        <v>42522</v>
+        <v>42521</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="17">
-        <v>42523</v>
+        <v>42522</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="17">
-        <v>42524</v>
+        <v>42523</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="17">
-        <v>42525</v>
+        <v>42524</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="17">
-        <v>42526</v>
+        <v>42525</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="17">
-        <v>42527</v>
+        <v>42526</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="17">
-        <v>42528</v>
+        <v>42527</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="17">
-        <v>42529</v>
+        <v>42528</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="17">
-        <v>42530</v>
+        <v>42529</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="17">
-        <v>42531</v>
+        <v>42530</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="17">
-        <v>42532</v>
+        <v>42531</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="17">
-        <v>42533</v>
+        <v>42532</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="17">
-        <v>42534</v>
+        <v>42533</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="17">
-        <v>42535</v>
+        <v>42534</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="17">
-        <v>42536</v>
+        <v>42535</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="17">
-        <v>42537</v>
+        <v>42536</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="17">
-        <v>42538</v>
+        <v>42537</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="17">
-        <v>42539</v>
+        <v>42538</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="17">
-        <v>42540</v>
+        <v>42539</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="17">
-        <v>42541</v>
+        <v>42540</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="17">
-        <v>42542</v>
+        <v>42541</v>
       </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="17">
-        <v>42543</v>
+        <v>42542</v>
       </c>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="17">
-        <v>42544</v>
+        <v>42543</v>
       </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="17">
-        <v>42545</v>
+        <v>42544</v>
       </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="17">
-        <v>42546</v>
+        <v>42545</v>
       </c>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="17">
-        <v>42547</v>
+        <v>42546</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="17">
-        <v>42548</v>
+        <v>42547</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="17">
-        <v>42549</v>
+        <v>42548</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="17">
-        <v>42550</v>
+        <v>42549</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="17">
-        <v>42551</v>
+        <v>42550</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="17">
-        <v>42552</v>
+        <v>42551</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="17">
-        <v>42553</v>
+        <v>42552</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="17">
-        <v>42554</v>
+        <v>42553</v>
       </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="17">
-        <v>42555</v>
+        <v>42554</v>
       </c>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="17">
-        <v>42556</v>
+        <v>42555</v>
       </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="17">
-        <v>42557</v>
+        <v>42556</v>
       </c>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="17">
-        <v>42558</v>
+        <v>42557</v>
       </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="17">
-        <v>42559</v>
+        <v>42558</v>
       </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="17">
-        <v>42560</v>
+        <v>42559</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="17">
-        <v>42561</v>
+        <v>42560</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="17">
+        <v>42561</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366" s="17">
         <v>42562</v>
       </c>
     </row>

</xml_diff>